<commit_message>
trigger  in rows with an empty stdX/YName/Unit
</commit_message>
<xml_diff>
--- a/data_preparation/rawDataUnique.xlsx
+++ b/data_preparation/rawDataUnique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duke\2021REU\nanomineParser\data_preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1385EB08-4E8D-47E4-84ED-BBE0A68BBB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F6D4EA-0B63-4B46-B45C-DC400C79CDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1222" yWindow="-98" windowWidth="18076" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8627" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8638" uniqueCount="1322">
   <si>
     <t>file</t>
   </si>
@@ -4843,12 +4843,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q638"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F177" sqref="F177"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8589,7 +8590,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>685</v>
       </c>
@@ -8615,7 +8616,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>685</v>
       </c>
@@ -10039,7 +10040,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>298</v>
       </c>
@@ -12142,7 +12143,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>660</v>
       </c>
@@ -12412,7 +12413,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>719</v>
       </c>
@@ -12454,6 +12455,9 @@
       </c>
       <c r="O164" t="s">
         <v>1218</v>
+      </c>
+      <c r="P164" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.45">
@@ -12829,7 +12833,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>927</v>
       </c>
@@ -13857,7 +13861,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>133</v>
       </c>
@@ -14864,7 +14868,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>242</v>
       </c>
@@ -14955,7 +14959,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>418</v>
       </c>
@@ -15087,7 +15091,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>788</v>
       </c>
@@ -15557,7 +15561,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>612</v>
       </c>
@@ -16162,7 +16166,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>612</v>
       </c>
@@ -16212,7 +16216,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>612</v>
       </c>
@@ -16262,7 +16266,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>701</v>
       </c>
@@ -16291,7 +16295,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>685</v>
       </c>
@@ -16317,7 +16321,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>685</v>
       </c>
@@ -18469,7 +18473,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>626</v>
       </c>
@@ -19194,7 +19198,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
         <v>898</v>
       </c>
@@ -19288,7 +19292,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>819</v>
       </c>
@@ -19329,7 +19333,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>819</v>
       </c>
@@ -19464,7 +19468,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
         <v>660</v>
       </c>
@@ -19505,7 +19509,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>660</v>
       </c>
@@ -20101,7 +20105,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A332" t="s">
         <v>107</v>
       </c>
@@ -20612,7 +20616,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>719</v>
       </c>
@@ -20650,7 +20654,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="344" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>523</v>
       </c>
@@ -20694,7 +20698,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>769</v>
       </c>
@@ -20741,7 +20745,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>678</v>
       </c>
@@ -20783,6 +20787,9 @@
       </c>
       <c r="O346" t="s">
         <v>1318</v>
+      </c>
+      <c r="P346" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="347" spans="1:16" x14ac:dyDescent="0.45">
@@ -20879,7 +20886,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="349" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>523</v>
       </c>
@@ -20917,7 +20924,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="350" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>523</v>
       </c>
@@ -20955,7 +20962,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>523</v>
       </c>
@@ -21137,7 +21144,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="355" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>467</v>
       </c>
@@ -21269,7 +21276,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="358" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
         <v>839</v>
       </c>
@@ -21410,7 +21417,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="361" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>701</v>
       </c>
@@ -21448,7 +21455,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="362" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A362" t="s">
         <v>698</v>
       </c>
@@ -21495,7 +21502,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="363" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
         <v>701</v>
       </c>
@@ -21542,7 +21549,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="364" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A364" t="s">
         <v>701</v>
       </c>
@@ -22238,7 +22245,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A379" t="s">
         <v>167</v>
       </c>
@@ -22291,7 +22298,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A380" t="s">
         <v>167</v>
       </c>
@@ -22438,7 +22445,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A383" t="s">
         <v>507</v>
       </c>
@@ -22485,7 +22492,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
       <c r="A384" t="s">
         <v>520</v>
       </c>
@@ -22532,7 +22539,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="385" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A385" t="s">
         <v>507</v>
       </c>
@@ -22579,7 +22586,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="386" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A386" t="s">
         <v>520</v>
       </c>
@@ -22996,7 +23003,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="395" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A395" t="s">
         <v>709</v>
       </c>
@@ -23046,7 +23053,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="396" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A396" t="s">
         <v>740</v>
       </c>
@@ -23510,7 +23517,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="406" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A406" t="s">
         <v>238</v>
       </c>
@@ -23547,8 +23554,11 @@
       <c r="O406" t="s">
         <v>1318</v>
       </c>
-    </row>
-    <row r="407" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P406" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="407" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A407" t="s">
         <v>761</v>
       </c>
@@ -23639,7 +23649,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="409" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A409" t="s">
         <v>752</v>
       </c>
@@ -23733,7 +23743,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="411" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A411" t="s">
         <v>372</v>
       </c>
@@ -23830,7 +23840,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="413" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A413" t="s">
         <v>377</v>
       </c>
@@ -24009,7 +24019,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="417" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A417" t="s">
         <v>715</v>
       </c>
@@ -24138,7 +24148,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="420" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A420" t="s">
         <v>701</v>
       </c>
@@ -24176,7 +24186,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="421" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A421" t="s">
         <v>701</v>
       </c>
@@ -24396,7 +24406,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="426" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A426" t="s">
         <v>564</v>
       </c>
@@ -24816,7 +24826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="435" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A435" t="s">
         <v>507</v>
       </c>
@@ -25133,7 +25143,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="442" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="442" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A442" t="s">
         <v>97</v>
       </c>
@@ -25169,6 +25179,9 @@
       </c>
       <c r="O442" t="s">
         <v>118</v>
+      </c>
+      <c r="P442" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="443" spans="1:16" x14ac:dyDescent="0.45">
@@ -25400,7 +25413,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="448" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A448" t="s">
         <v>97</v>
       </c>
@@ -25436,6 +25449,9 @@
       </c>
       <c r="O448" t="s">
         <v>342</v>
+      </c>
+      <c r="P448" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="449" spans="1:16" x14ac:dyDescent="0.45">
@@ -25717,7 +25733,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="455" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A455" t="s">
         <v>752</v>
       </c>
@@ -25814,7 +25830,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="457" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A457" t="s">
         <v>728</v>
       </c>
@@ -25905,7 +25921,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="459" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A459" t="s">
         <v>97</v>
       </c>
@@ -26046,7 +26062,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="462" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A462" t="s">
         <v>733</v>
       </c>
@@ -26137,7 +26153,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="464" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A464" t="s">
         <v>315</v>
       </c>
@@ -26175,7 +26191,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="465" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A465" t="s">
         <v>535</v>
       </c>
@@ -26216,7 +26232,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="466" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A466" t="s">
         <v>535</v>
       </c>
@@ -26257,7 +26273,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="467" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A467" t="s">
         <v>382</v>
       </c>
@@ -26286,7 +26302,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="468" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="468" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A468" t="s">
         <v>535</v>
       </c>
@@ -26327,7 +26343,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="469" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A469" t="s">
         <v>543</v>
       </c>
@@ -26353,7 +26369,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="470" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="470" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A470" t="s">
         <v>543</v>
       </c>
@@ -26379,7 +26395,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="471" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="471" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A471" t="s">
         <v>645</v>
       </c>
@@ -26423,7 +26439,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="472" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="472" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A472" t="s">
         <v>857</v>
       </c>
@@ -26470,7 +26486,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="473" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="473" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A473" t="s">
         <v>535</v>
       </c>
@@ -26511,7 +26527,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="474" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="474" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A474" t="s">
         <v>467</v>
       </c>
@@ -26593,7 +26609,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="476" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="476" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A476" t="s">
         <v>535</v>
       </c>
@@ -26681,7 +26697,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="478" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="478" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A478" t="s">
         <v>315</v>
       </c>
@@ -26713,7 +26729,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="479" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="479" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A479" t="s">
         <v>467</v>
       </c>
@@ -27230,7 +27246,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="490" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="490" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A490" t="s">
         <v>523</v>
       </c>
@@ -27274,7 +27290,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="491" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="491" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A491" t="s">
         <v>623</v>
       </c>
@@ -27368,7 +27384,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="493" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="493" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A493" t="s">
         <v>594</v>
       </c>
@@ -28073,7 +28089,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="508" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="508" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A508" t="s">
         <v>475</v>
       </c>
@@ -28164,7 +28180,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="510" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="510" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A510" t="s">
         <v>475</v>
       </c>
@@ -28289,6 +28305,9 @@
       <c r="K512" t="s">
         <v>1195</v>
       </c>
+      <c r="L512" t="s">
+        <v>349</v>
+      </c>
       <c r="M512" t="s">
         <v>1196</v>
       </c>
@@ -28333,6 +28352,9 @@
       <c r="K513" t="s">
         <v>1195</v>
       </c>
+      <c r="L513" t="s">
+        <v>349</v>
+      </c>
       <c r="M513" t="s">
         <v>1196</v>
       </c>
@@ -28377,6 +28399,9 @@
       <c r="K514" t="s">
         <v>1195</v>
       </c>
+      <c r="L514" t="s">
+        <v>349</v>
+      </c>
       <c r="M514" t="s">
         <v>1196</v>
       </c>
@@ -28421,6 +28446,9 @@
       <c r="K515" t="s">
         <v>1195</v>
       </c>
+      <c r="L515" t="s">
+        <v>349</v>
+      </c>
       <c r="M515" t="s">
         <v>1196</v>
       </c>
@@ -28478,7 +28506,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="517" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="517" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A517" t="s">
         <v>335</v>
       </c>
@@ -28516,7 +28544,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="518" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="518" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A518" t="s">
         <v>335</v>
       </c>
@@ -30004,7 +30032,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="551" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="551" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A551" t="s">
         <v>252</v>
       </c>
@@ -30040,6 +30068,9 @@
       </c>
       <c r="O551" t="s">
         <v>342</v>
+      </c>
+      <c r="P551" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="552" spans="1:16" x14ac:dyDescent="0.45">
@@ -30362,7 +30393,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="559" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="559" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A559" t="s">
         <v>364</v>
       </c>
@@ -30720,7 +30751,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="567" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="567" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A567" t="s">
         <v>719</v>
       </c>
@@ -31002,7 +31033,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="573" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="573" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A573" t="s">
         <v>735</v>
       </c>
@@ -31093,7 +31124,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="575" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="575" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A575" t="s">
         <v>208</v>
       </c>
@@ -31137,7 +31168,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="576" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="576" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A576" t="s">
         <v>784</v>
       </c>
@@ -31272,7 +31303,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="579" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="579" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A579" t="s">
         <v>784</v>
       </c>
@@ -31298,7 +31329,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="580" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="580" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A580" t="s">
         <v>364</v>
       </c>
@@ -31345,7 +31376,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="581" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="581" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A581" t="s">
         <v>177</v>
       </c>
@@ -31430,7 +31461,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="583" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="583" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A583" t="s">
         <v>543</v>
       </c>
@@ -31456,7 +31487,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="584" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="584" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A584" t="s">
         <v>548</v>
       </c>
@@ -31482,7 +31513,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="585" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="585" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A585" t="s">
         <v>489</v>
       </c>
@@ -31529,7 +31560,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="586" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="586" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A586" t="s">
         <v>377</v>
       </c>
@@ -31605,7 +31636,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="588" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="588" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A588" t="s">
         <v>523</v>
       </c>
@@ -31646,7 +31677,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="589" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="589" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A589" t="s">
         <v>533</v>
       </c>
@@ -31687,7 +31718,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="590" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="590" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A590" t="s">
         <v>505</v>
       </c>
@@ -31728,7 +31759,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="591" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="591" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A591" t="s">
         <v>271</v>
       </c>
@@ -31772,7 +31803,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="592" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="592" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A592" t="s">
         <v>271</v>
       </c>
@@ -31816,7 +31847,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="593" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="593" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A593" t="s">
         <v>812</v>
       </c>
@@ -31860,7 +31891,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="594" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="594" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A594" t="s">
         <v>813</v>
       </c>
@@ -32004,7 +32035,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="597" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="597" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A597" t="s">
         <v>805</v>
       </c>
@@ -32127,7 +32158,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="600" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="600" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A600" t="s">
         <v>482</v>
       </c>
@@ -32171,7 +32202,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="601" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="601" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A601" t="s">
         <v>475</v>
       </c>
@@ -32214,8 +32245,11 @@
       <c r="O601" t="s">
         <v>982</v>
       </c>
-    </row>
-    <row r="602" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P601" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="602" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A602" t="s">
         <v>693</v>
       </c>
@@ -32309,7 +32343,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="604" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="604" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A604" t="s">
         <v>693</v>
       </c>
@@ -32823,7 +32857,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="615" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="615" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A615" t="s">
         <v>862</v>
       </c>
@@ -33943,7 +33977,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q638" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q638" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="15">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P653">
     <sortCondition descending="1" ref="C2:C653"/>
     <sortCondition ref="B2:B653"/>

</xml_diff>